<commit_message>
up nhan exxcel gia dat dia ban p1
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaDatDiaBan.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaDatDiaBan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\ASP\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4961B95-47C2-4F3F-8E9C-15AB7574F86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B3D9E0-7842-48D0-A62B-7B6A9DAFCE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11310" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,46 +25,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
-  <si>
-    <t>Phân loại</t>
-  </si>
-  <si>
-    <t>Giá</t>
-  </si>
-  <si>
-    <t>Đơn vị</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>Mã nhóm</t>
-  </si>
-  <si>
-    <t>Nhà có khu phụ</t>
-  </si>
-  <si>
-    <t>Nhà không có khu phụ</t>
-  </si>
-  <si>
-    <t>Nhà khác</t>
-  </si>
-  <si>
-    <t>Tên nhóm</t>
-  </si>
-  <si>
-    <t>Nhà 1 tầng, tường 111</t>
-  </si>
-  <si>
-    <t>Nhà 1 tầng, tường 200</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Tên đường</t>
+  </si>
+  <si>
+    <t>Điểm đầu</t>
+  </si>
+  <si>
+    <t>Điểm cuối</t>
+  </si>
+  <si>
+    <t>Hệ số</t>
+  </si>
+  <si>
+    <t>Giá đất theo hệ số đường</t>
+  </si>
+  <si>
+    <t>VT1</t>
+  </si>
+  <si>
+    <t>VT2</t>
+  </si>
+  <si>
+    <t>VT3</t>
+  </si>
+  <si>
+    <t>VT4</t>
+  </si>
+  <si>
+    <t>VT5</t>
+  </si>
+  <si>
+    <t>An Dương Vương</t>
+  </si>
+  <si>
+    <t>Nguyễn Trãi</t>
+  </si>
+  <si>
+    <t>Trần Khánh Dư</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảng giá đất </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +98,29 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,22 +138,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0BC2B6-4560-4170-B0EA-9A729F87B874}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,127 +523,147 @@
     <col min="5" max="5" width="38.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>231130563414</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>231130563414</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>231130224114</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>231130224114</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>231130224114</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="B4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="11">
+        <v>8100000</v>
+      </c>
+      <c r="G4" s="11">
+        <v>4860000</v>
+      </c>
+      <c r="H4" s="11">
+        <v>4050000</v>
+      </c>
+      <c r="I4" s="11">
+        <v>2025000</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1080000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>